<commit_message>
chore: update endpoint for get user list and import users from file
</commit_message>
<xml_diff>
--- a/resources/account-example.xlsx
+++ b/resources/account-example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonhoang/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\ez-exam-fe\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DFA57E1-D3B9-2D46-9C66-CA6DFA862A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960B9591-DC56-497B-BD47-9CC47C9D15D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{868544FC-A559-5C49-818D-FF161B1E2031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{868544FC-A559-5C49-818D-FF161B1E2031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,26 +20,14 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>tenNguoiDung</t>
-  </si>
-  <si>
-    <t>matKhau</t>
   </si>
   <si>
     <t>loai</t>
@@ -64,18 +52,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,16 +78,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -420,20 +397,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2C8CD4-2133-224E-9A7B-C857A9A76A1E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,42 +419,30 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>123123123</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
-      </c>
-      <c r="B3">
-        <v>222222</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="test7@gmail.com" xr:uid="{71DA78FB-7D9D-CC4F-9104-A9E0F7C7DC9F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: update admin account creation/edit screen, comment out add to question list button
</commit_message>
<xml_diff>
--- a/resources/account-example.xlsx
+++ b/resources/account-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\ez-exam-fe\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960B9591-DC56-497B-BD47-9CC47C9D15D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914CB3D2-6576-4B8D-8DE1-F7B77BE06583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{868544FC-A559-5C49-818D-FF161B1E2031}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>tenNguoiDung</t>
   </si>
@@ -46,16 +46,33 @@
   </si>
   <si>
     <t>test72</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>test_email@gmail.com</t>
+  </si>
+  <si>
+    <t>admin@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +95,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,52 +417,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2C8CD4-2133-224E-9A7B-C857A9A76A1E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.125" customWidth="1"/>
-    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="1" max="2" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F6C8E7CA-845F-45B8-B496-D4995304F2E2}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{CBCA1B2F-FB6F-43B7-98FA-BCF070011FCF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: add account info screen, change excel demo file
</commit_message>
<xml_diff>
--- a/resources/account-example.xlsx
+++ b/resources/account-example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\ez-exam-fe\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914CB3D2-6576-4B8D-8DE1-F7B77BE06583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05349B5A-4437-451B-AE36-57E1DFE4626B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{868544FC-A559-5C49-818D-FF161B1E2031}"/>
   </bookViews>
@@ -420,13 +420,14 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.125" customWidth="1"/>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="1" max="1" width="20.125" customWidth="1"/>
+    <col min="2" max="2" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="20.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -434,47 +435,47 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F6C8E7CA-845F-45B8-B496-D4995304F2E2}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{CBCA1B2F-FB6F-43B7-98FA-BCF070011FCF}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{F6C8E7CA-845F-45B8-B496-D4995304F2E2}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{CBCA1B2F-FB6F-43B7-98FA-BCF070011FCF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>